<commit_message>
map edit finished, prepare to modify data node structure
</commit_message>
<xml_diff>
--- a/qins_moon/res/tables/test/core/politics.xlsx
+++ b/qins_moon/res/tables/test/core/politics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28451" windowHeight="8904" tabRatio="954" firstSheet="4" activeTab="20"/>
+    <workbookView windowWidth="21431" windowHeight="11268" tabRatio="954"/>
   </bookViews>
   <sheets>
     <sheet name="TerrainTerrain" sheetId="2" r:id="rId1"/>
@@ -553,11 +553,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -583,35 +583,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -620,9 +591,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,84 +614,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -728,9 +632,105 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -743,49 +743,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,19 +755,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,7 +791,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,13 +833,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,73 +911,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,11 +937,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -961,11 +978,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -994,42 +1017,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1038,137 +1038,137 @@
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1512,8 +1512,8 @@
   <sheetPr/>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.537037037037" defaultRowHeight="13.2" outlineLevelCol="6"/>
@@ -2661,7 +2661,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.537037037037" defaultRowHeight="13.2" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -2878,7 +2878,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.537037037037" defaultRowHeight="13.2" outlineLevelRow="1"/>
@@ -3193,7 +3193,7 @@
   <dimension ref="A5:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.537037037037" defaultRowHeight="13.2"/>
@@ -3500,7 +3500,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.537037037037" defaultRowHeight="13.2" outlineLevelCol="3"/>
@@ -3880,7 +3880,7 @@
   <sheetPr/>
   <dimension ref="A5:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -3965,7 +3965,7 @@
   <dimension ref="A5:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.2" outlineLevelRow="5" outlineLevelCol="3"/>

</xml_diff>